<commit_message>
Update classifier, UI defaults, docs; run ruff and black
</commit_message>
<xml_diff>
--- a/data/seed/rave_export_demo.xlsx
+++ b/data/seed/rave_export_demo.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,192 +767,351 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>listing</t>
+          <t>edit_check</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>SUBJ-1007</t>
+          <t>SUBJ-1008</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>DMWEIGHT, DMWTU</t>
+          <t>AEENDTC</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Inconsistent units: weight in kg vs lb across visits.</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>Missing end date for ongoing AE.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2024-01-20</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>DMWTU</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>lb</t>
-        </is>
-      </c>
+          <t>AEENDTC</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Study standard kg</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Previous visit was kg</t>
-        </is>
-      </c>
+          <t>Required when AEOUT=Ongoing</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>edit_check</t>
+          <t>listing</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>SUBJ-1008</t>
+          <t>SUBJ-1009</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>AEENDTC</t>
+          <t>LBORRES, LBCLSIG</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Missing end date for ongoing AE.</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2024-01-20</t>
-        </is>
-      </c>
+          <t>Discrepancy vs central lab: EDC value differs from external. Clinical significance unclear.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>AEENDTC</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr"/>
+          <t>LBORRES</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>12.5</t>
+        </is>
+      </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Required when AEOUT=Ongoing</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr"/>
+          <t>Central lab 11.8</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>LBCLSIG=Y, requires clinical context</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>listing</t>
+          <t>edit_check</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>DM</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>SUBJ-1009</t>
+          <t>SUBJ-1010</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>LBORRES, LBCLSIG</t>
+          <t>BRTHDTC</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Discrepancy vs central lab: EDC value differs from external.</t>
+          <t>Invalid or partial date: birth date month/year only. May be acceptable per protocol.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>LBORRES</t>
+          <t>BRTHDTC</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>12.5</t>
+          <t>1985-03</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Central lab 11.8</t>
+          <t>ISO 8601 full date</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>LBCLSIG=Y</t>
+          <t>Partial date may be acceptable</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>edit_check</t>
+          <t>listing</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>SUBJ-1010</t>
+          <t>SUBJ-1011</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>BRTHDTC</t>
+          <t>AETERM, AESEV, AESER</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Invalid or partial date: birth date month/year only.</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
+          <t>Complex adverse event with multiple related conditions. Requires medical review to determine if single or multiple events.</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2024-04-10</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>BRTHDTC</t>
+          <t>AETERM</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1985-03</t>
+          <t>Headache, Nausea, Dizziness</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>ISO 8601 full date</t>
+          <t>Multiple symptoms</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Partial date not allowed</t>
+          <t>Need to assess if related or separate</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>listing</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DM</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>SUBJ-1012</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>DMWEIGHT, DMWTU</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Inconsistent units: weight in kg vs lb across visits. Need to assess impact on BMI calculations.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>DMWTU</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>lb</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Study standard kg</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Previous visit was kg, BMI affected</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>edit_check</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>AE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>SUBJ-1013</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>AESTDTC, AEENDTC, AESER</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Serious adverse event with ambiguous timeline. Start date conflicts with hospitalization records.</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2024-05-01</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>AESTDTC</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2024-05-03</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Hospitalization started 2024-05-03</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Date reconciliation needed</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>listing</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SUBJ-1014</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>CMTRT, CMDOSFRM</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Uncommon medication coding issue: combination product not in standard dictionary. Requires manual review.</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>CMTRT</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Product-XY Plus</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Not in MedDRA/WHODrug</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Novel combination product</t>
         </is>
       </c>
     </row>

</xml_diff>